<commit_message>
introduced new classes, created person class with preferences. Moving towards objects
</commit_message>
<xml_diff>
--- a/Shift/sheets/Responses.xlsx
+++ b/Shift/sheets/Responses.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Timestamp</t>
   </si>
@@ -193,12 +193,15 @@
   </si>
   <si>
     <t>FRI 8PM-12AM, SAT 12PM-4PM, SAT4PM-8PM, SAT 8PM-12AM, SUN 12PM-4PM, SUN 4PM-8PM, SUN 8PM-12AM</t>
+  </si>
+  <si>
+    <t>Seniority</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -557,12 +560,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -570,7 +573,7 @@
     <col min="1" max="3" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,8 +583,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42519.602106909719</v>
       </c>
@@ -591,8 +597,11 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>42519.602299895836</v>
       </c>
@@ -602,8 +611,11 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42519.602701145835</v>
       </c>
@@ -613,8 +625,11 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42519.603819085649</v>
       </c>
@@ -624,8 +639,11 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42519.604019629631</v>
       </c>
@@ -635,8 +653,11 @@
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42519.607258240736</v>
       </c>
@@ -646,8 +667,11 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42519.607830138892</v>
       </c>
@@ -657,8 +681,11 @@
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>42519.607868368053</v>
       </c>
@@ -668,8 +695,11 @@
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42519.612853784725</v>
       </c>
@@ -679,8 +709,11 @@
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>42519.61306993055</v>
       </c>
@@ -690,8 +723,11 @@
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>42519.620290937499</v>
       </c>
@@ -701,8 +737,11 @@
       <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>42519.624560879631</v>
       </c>
@@ -712,8 +751,11 @@
       <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42519.627129780092</v>
       </c>
@@ -723,8 +765,11 @@
       <c r="C14" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42519.641950960649</v>
       </c>
@@ -734,8 +779,11 @@
       <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>42519.646164687496</v>
       </c>
@@ -745,8 +793,11 @@
       <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>42519.657218888889</v>
       </c>
@@ -756,8 +807,11 @@
       <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>42519.722283414347</v>
       </c>
@@ -767,8 +821,11 @@
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>42519.772954479165</v>
       </c>
@@ -778,8 +835,11 @@
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>42519.800402118053</v>
       </c>
@@ -789,8 +849,11 @@
       <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>42520.612079189814</v>
       </c>
@@ -800,8 +863,11 @@
       <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>42520.712805821764</v>
       </c>
@@ -811,8 +877,11 @@
       <c r="C22" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>42520.992902696758</v>
       </c>
@@ -822,8 +891,11 @@
       <c r="C23" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>42521.470976643519</v>
       </c>
@@ -833,8 +905,11 @@
       <c r="C24" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>42521.731479212962</v>
       </c>
@@ -844,8 +919,11 @@
       <c r="C25" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>42521.893794537042</v>
       </c>
@@ -855,8 +933,11 @@
       <c r="C26" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42521.908353171297</v>
       </c>
@@ -866,8 +947,11 @@
       <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42522.511084189813</v>
       </c>
@@ -877,8 +961,11 @@
       <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>42524.799749826387</v>
       </c>
@@ -887,6 +974,9 @@
       </c>
       <c r="C29" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to dataprocessing. starting to parse data
</commit_message>
<xml_diff>
--- a/Shift/sheets/Responses.xlsx
+++ b/Shift/sheets/Responses.xlsx
@@ -192,10 +192,10 @@
     <t>Ilya Verzhbinsky</t>
   </si>
   <si>
-    <t>FRI 8PM-12AM, SAT 12PM-4PM, SAT4PM-8PM, SAT 8PM-12AM, SUN 12PM-4PM, SUN 4PM-8PM, SUN 8PM-12AM</t>
-  </si>
-  <si>
     <t>Seniority</t>
+  </si>
+  <si>
+    <t>FRI 8PM-12AM, SAT 12PM-4PM, SAT 4PM-8PM, SAT 8PM-12AM, SUN 12PM-4PM, SUN 4PM-8PM, SUN 8PM-12AM</t>
   </si>
 </sst>
 </file>
@@ -563,14 +563,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.54296875" customWidth="1"/>
+    <col min="1" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="186.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -584,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -973,7 +974,7 @@
         <v>56</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D29">
         <v>4</v>

</xml_diff>

<commit_message>
got person class working with preferences
</commit_message>
<xml_diff>
--- a/Shift/sheets/Responses.xlsx
+++ b/Shift/sheets/Responses.xlsx
@@ -39,9 +39,6 @@
     <t>Hannah McElroy</t>
   </si>
   <si>
-    <t>MON 8AM -12PM, MON 12PM-4PM, MON 4PM-8PM, MON 8PM-12AM, TUES 8AM-12PM, TUES 12PM-4PM, TUES 4PM-8PM, TUES 8PM-12AM, WEDS 8AM-12PM, WEDS 12PM-4PM, WEDS 4PM-8PM, WEDS 8PM-12AM</t>
-  </si>
-  <si>
     <t>corinne rezentes</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Steven Tohmasi</t>
   </si>
   <si>
-    <t>SAT 12PM-4PM, SAT4PM-8PM, SAT 8PM-12AM, SUN 12PM-4PM, SUN 4PM-8PM</t>
-  </si>
-  <si>
     <t>Linsay ling</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>Victoria Stoffers</t>
   </si>
   <si>
-    <t>MON 8AM -12PM, MON 12PM-4PM, TUES 8AM-12PM, TUES 12PM-4PM, FRI 8AM-12PM, FRI 12PM-4PM</t>
-  </si>
-  <si>
     <t>Karen Bryan</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>Jessie Van Fleet</t>
   </si>
   <si>
-    <t>MON 8AM -12PM, MON 12PM-4PM, MON 4PM-8PM, TUES 8AM-12PM, TUES 12PM-4PM</t>
-  </si>
-  <si>
     <t>Paras Shah</t>
   </si>
   <si>
@@ -156,9 +144,6 @@
     <t>Justin De La Guerra</t>
   </si>
   <si>
-    <t>, MON 12PM-4PM, MON 4PM-8PM, MON 8PM-12AM, TUES 8AM-12PM</t>
-  </si>
-  <si>
     <t>Donald Chow</t>
   </si>
   <si>
@@ -180,15 +165,9 @@
     <t>Sydney Swanson (preferably Tuesday :) )</t>
   </si>
   <si>
-    <t>MON 8AM -12PM, MON 12PM-4PM, MON 4PM-8PM, TUES 4PM-8PM, SUN 8PM-12AM</t>
-  </si>
-  <si>
     <t>Hunter Hu</t>
   </si>
   <si>
-    <t>MON 8AM -12PM, MON 12PM-4PM, TUES 8AM-12PM, TUES 12PM-4PM, TUES 4PM-8PM, TUES 8PM-12AM, WEDS 8AM-12PM, WEDS 12PM-4PM</t>
-  </si>
-  <si>
     <t>Ilya Verzhbinsky</t>
   </si>
   <si>
@@ -196,6 +175,27 @@
   </si>
   <si>
     <t>FRI 8PM-12AM, SAT 12PM-4PM, SAT 4PM-8PM, SAT 8PM-12AM, SUN 12PM-4PM, SUN 4PM-8PM, SUN 8PM-12AM</t>
+  </si>
+  <si>
+    <t>MON 8AM-12PM, MON 12PM-4PM, MON 4PM-8PM, MON 8PM-12AM, TUES 8AM-12PM, TUES 12PM-4PM, TUES 4PM-8PM, TUES 8PM-12AM, WEDS 8AM-12PM, WEDS 12PM-4PM, WEDS 4PM-8PM, WEDS 8PM-12AM</t>
+  </si>
+  <si>
+    <t>MON 8AM-12PM, MON 12PM-4PM, TUES 8AM-12PM, TUES 12PM-4PM, FRI 8AM-12PM, FRI 12PM-4PM</t>
+  </si>
+  <si>
+    <t>MON 8AM-12PM, MON 12PM-4PM, MON 4PM-8PM, TUES 8AM-12PM, TUES 12PM-4PM</t>
+  </si>
+  <si>
+    <t>MON 8AM-12PM, MON 12PM-4PM, MON 4PM-8PM, TUES 4PM-8PM, SUN 8PM-12AM</t>
+  </si>
+  <si>
+    <t>MON 8AM-12PM, MON 12PM-4PM, TUES 8AM-12PM, TUES 12PM-4PM, TUES 4PM-8PM, TUES 8PM-12AM, WEDS 8AM-12PM, WEDS 12PM-4PM</t>
+  </si>
+  <si>
+    <t>SAT 12PM-4PM, SAT 4PM-8PM, SAT 8PM-12AM, SUN 12PM-4PM, SUN 4PM-8PM</t>
+  </si>
+  <si>
+    <t>MON 12PM-4PM, MON 4PM-8PM, MON 8PM-12AM, TUES 8AM-12PM</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +220,11 @@
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,11 +247,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -585,7 +591,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -610,7 +616,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -621,10 +627,10 @@
         <v>42519.602701145835</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -635,10 +641,10 @@
         <v>42519.603819085649</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -649,10 +655,10 @@
         <v>42519.604019629631</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -663,10 +669,10 @@
         <v>42519.607258240736</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -677,10 +683,10 @@
         <v>42519.607830138892</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -691,10 +697,10 @@
         <v>42519.607868368053</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -705,10 +711,10 @@
         <v>42519.612853784725</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -719,10 +725,10 @@
         <v>42519.61306993055</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -733,10 +739,10 @@
         <v>42519.620290937499</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -747,10 +753,10 @@
         <v>42519.624560879631</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -761,10 +767,10 @@
         <v>42519.627129780092</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -775,10 +781,10 @@
         <v>42519.641950960649</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -789,10 +795,10 @@
         <v>42519.646164687496</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -803,10 +809,10 @@
         <v>42519.657218888889</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -817,10 +823,10 @@
         <v>42519.722283414347</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -831,10 +837,10 @@
         <v>42519.772954479165</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -845,10 +851,10 @@
         <v>42519.800402118053</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -859,10 +865,10 @@
         <v>42520.612079189814</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -873,10 +879,10 @@
         <v>42520.712805821764</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -887,10 +893,10 @@
         <v>42520.992902696758</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -901,10 +907,10 @@
         <v>42521.470976643519</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -915,10 +921,10 @@
         <v>42521.731479212962</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -929,10 +935,10 @@
         <v>42521.893794537042</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -943,10 +949,10 @@
         <v>42521.908353171297</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -957,10 +963,10 @@
         <v>42522.511084189813</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -971,10 +977,10 @@
         <v>42524.799749826387</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -982,5 +988,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
calendar ordering system sort of works
</commit_message>
<xml_diff>
--- a/Shift/sheets/Responses.xlsx
+++ b/Shift/sheets/Responses.xlsx
@@ -569,9 +569,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -647,7 +647,7 @@
         <v>57</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>14</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>18</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -745,7 +745,7 @@
         <v>21</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -759,7 +759,7 @@
         <v>23</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -787,7 +787,7 @@
         <v>27</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
         <v>30</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -843,7 +843,7 @@
         <v>54</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -871,7 +871,7 @@
         <v>37</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>39</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -899,7 +899,7 @@
         <v>58</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>42</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -927,7 +927,7 @@
         <v>44</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -969,7 +969,7 @@
         <v>56</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -983,7 +983,7 @@
         <v>51</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>